<commit_message>
Central Limit theorem revision
</commit_message>
<xml_diff>
--- a/ISB Examples/Statistics/Worksheets for calculations.xlsx
+++ b/ISB Examples/Statistics/Worksheets for calculations.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandipto.sanyal\OneDrive - Accenture\Documents\Study materials\self study\self_study\Statistics Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandipto.sanyal\OneDrive - Accenture\Documents\Study materials\self study\self_study\ISB Examples\Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="11_F25DC773A252ABDACC104838D99C643C5BDE58F3" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AB4697A6-BED6-483C-86C2-C905E85027C7}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="11_F25DC773A252ABDACC104838D99C643C5BDE58F3" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CFBC60DF-1709-43DF-9CFD-6E9AAB7358AF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cricketer Bayes theorem" sheetId="1" r:id="rId1"/>
+    <sheet name="Visualize CLT" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cricketer Bayes theorem'!$A$1:$I$12</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
   <si>
     <t>Smokes</t>
   </si>
@@ -75,13 +76,169 @@
   </si>
   <si>
     <t>P(Not Character | Not Cricketer)</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>P14</t>
+  </si>
+  <si>
+    <t>P15</t>
+  </si>
+  <si>
+    <t>P16</t>
+  </si>
+  <si>
+    <t>P17</t>
+  </si>
+  <si>
+    <t>P18</t>
+  </si>
+  <si>
+    <t>P19</t>
+  </si>
+  <si>
+    <t>P20</t>
+  </si>
+  <si>
+    <t>P21</t>
+  </si>
+  <si>
+    <t>P22</t>
+  </si>
+  <si>
+    <t>P23</t>
+  </si>
+  <si>
+    <t>P24</t>
+  </si>
+  <si>
+    <t>P25</t>
+  </si>
+  <si>
+    <t>P26</t>
+  </si>
+  <si>
+    <t>P27</t>
+  </si>
+  <si>
+    <t>P28</t>
+  </si>
+  <si>
+    <t>P29</t>
+  </si>
+  <si>
+    <t>P30</t>
+  </si>
+  <si>
+    <t>P31</t>
+  </si>
+  <si>
+    <t>P32</t>
+  </si>
+  <si>
+    <t>P33</t>
+  </si>
+  <si>
+    <t>P34</t>
+  </si>
+  <si>
+    <t>P35</t>
+  </si>
+  <si>
+    <t>P36</t>
+  </si>
+  <si>
+    <t>P37</t>
+  </si>
+  <si>
+    <t>P38</t>
+  </si>
+  <si>
+    <t>P39</t>
+  </si>
+  <si>
+    <t>P40</t>
+  </si>
+  <si>
+    <t>P41</t>
+  </si>
+  <si>
+    <t>P42</t>
+  </si>
+  <si>
+    <t>P43</t>
+  </si>
+  <si>
+    <t>P44</t>
+  </si>
+  <si>
+    <t>P45</t>
+  </si>
+  <si>
+    <t>P46</t>
+  </si>
+  <si>
+    <t>P47</t>
+  </si>
+  <si>
+    <t>P48</t>
+  </si>
+  <si>
+    <t>P49</t>
+  </si>
+  <si>
+    <t>P50</t>
+  </si>
+  <si>
+    <t>Person names</t>
+  </si>
+  <si>
+    <t>Person age</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +250,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -525,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -799,4 +962,478 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915CF36F-BFC8-4BA1-971F-3C1F50894C34}">
+  <dimension ref="A1:B51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="B148" sqref="B148"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <f ca="1">RANDBETWEEN(0,100)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B66" ca="1" si="0">RANDBETWEEN(0,100)</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ca="1" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ca="1" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ca="1" si="0"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ca="1" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ca="1" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26">
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28">
+        <f t="shared" ca="1" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29">
+        <f t="shared" ca="1" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31">
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32">
+        <f t="shared" ca="1" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ca="1" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35">
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36">
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37">
+        <f t="shared" ca="1" si="0"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39">
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40">
+        <f t="shared" ca="1" si="0"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41">
+        <f t="shared" ca="1" si="0"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42">
+        <f t="shared" ca="1" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44">
+        <f t="shared" ca="1" si="0"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45">
+        <f t="shared" ca="1" si="0"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46">
+        <f t="shared" ca="1" si="0"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47">
+        <f t="shared" ca="1" si="0"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49">
+        <f t="shared" ca="1" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50">
+        <f t="shared" ca="1" si="0"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51">
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>